<commit_message>
ExportToXL solution Update for: if no file if file exist but empty ExcelSheet Initialization
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/TestOutput.xlsx
+++ b/target/test-classes/TestData/TestOutput.xlsx
@@ -3,36 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Git\SimpleTestCase\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
-    <sheet name="TestReport" sheetId="1" r:id="rId1"/>
+    <sheet name="TestReport 29-08-2022 21.18.42" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+  <si>
+    <t>Test Step</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Test Step</t>
   </si>
   <si>
     <t>Adım 1.</t>
@@ -82,28 +77,7 @@
 Açılan sayfada bir önceki sayfada beğendiklerime alınmış ürünün bulunduğunu onaylayacak</t>
   </si>
   <si>
-    <t>Adım 12 13</t>
-  </si>
-  <si>
-    <t>Beğendiklerime alınmış ürün bulunup seçilecek ve sepete eklenecek
-'Ürün sepete eklendi' popup kontrolü yapacak</t>
-  </si>
-  <si>
-    <t>Adım 14 15 16</t>
-  </si>
-  <si>
-    <t>Sepetim sayfasına gidecek
-Sepete eklenen bu ürünün içine girilip 'Kaldır' butonuna basılacak, sepetimden çıkarılacak
-Bu ürünün artik sepette olmadığını onaylayacak</t>
-  </si>
-  <si>
     <t>optiimMulakatTestiTesti</t>
-  </si>
-  <si>
-    <t>ITestResult=1ile Sonlanmıştır</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>ITestResult=2 ile Sonlanmıştır.</t>
@@ -119,20 +93,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,9 +122,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,28 +404,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.88671875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="255.77734375"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -536,59 +499,13 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>